<commit_message>
fixed legend sku-T2 NLS results
</commit_message>
<xml_diff>
--- a/results/Final Results GA vs. NLS.xlsx
+++ b/results/Final Results GA vs. NLS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="37">
   <si>
     <t>Path</t>
   </si>
@@ -52681,7 +52681,9 @@
         <v>23</v>
       </c>
       <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="33"/>
@@ -52706,7 +52708,9 @@
       <c r="J2" s="34"/>
       <c r="K2" s="34"/>
       <c r="L2" s="34"/>
-      <c r="M2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
@@ -52772,10 +52776,9 @@
       <c r="L4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="M4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="17"/>
@@ -52805,10 +52808,9 @@
         <v>3.0</v>
       </c>
       <c r="L5" s="34"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="M5" s="19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
@@ -70982,7 +70984,7 @@
       <c r="P968" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="60">
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="A33:A35"/>
@@ -71010,8 +71012,10 @@
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="M1:P1"/>
     <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="M5:P5"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>

</xml_diff>